<commit_message>
cleanups and added exclusion feature
</commit_message>
<xml_diff>
--- a/Data/UCH_Data.xlsx
+++ b/Data/UCH_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\uch-ranking\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D8E670-9C37-4DBE-ADB4-4BFB84BBF6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FEDAB2-E1AB-4746-9E58-52819D95AC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="-108" windowWidth="39528" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="-108" windowWidth="39528" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="77">
   <si>
     <t>Winner1</t>
   </si>
@@ -264,6 +264,12 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>Excluded</t>
+  </si>
+  <si>
+    <t>True</t>
   </si>
 </sst>
 </file>
@@ -750,9 +756,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -798,12 +805,11 @@
     <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="11">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <b/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -880,16 +886,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Players2__2" displayName="Players2__2" ref="A1:B32" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B32" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Players2__2" displayName="Players2__2" ref="A1:B32" tableType="queryTable" totalsRowShown="0" headerRowDxfId="0">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B32">
     <sortCondition ref="B1:B32"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="ShortName" queryTableFieldId="1" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="ShortName" queryTableFieldId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Name" queryTableFieldId="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -897,16 +902,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Matches2" displayName="Matches2" ref="A1:K162" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:K162" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" uniqueName="1" name="Winner1" queryTableFieldId="1" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" uniqueName="2" name="Winner2" queryTableFieldId="2" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" uniqueName="3" name="Winner3" queryTableFieldId="3" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" uniqueName="4" name="Winner4" queryTableFieldId="4" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" uniqueName="5" name="Winner5" queryTableFieldId="5" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" uniqueName="6" name="Loser1" queryTableFieldId="6" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" uniqueName="7" name="Loser2" queryTableFieldId="7" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" uniqueName="8" name="Loser3" queryTableFieldId="8" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" uniqueName="9" name="Loser4" queryTableFieldId="9" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" uniqueName="10" name="Loser5" queryTableFieldId="10" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" uniqueName="1" name="Winner1" queryTableFieldId="1" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" uniqueName="2" name="Winner2" queryTableFieldId="2" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" uniqueName="3" name="Winner3" queryTableFieldId="3" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" uniqueName="4" name="Winner4" queryTableFieldId="4" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" uniqueName="5" name="Winner5" queryTableFieldId="5" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" uniqueName="6" name="Loser1" queryTableFieldId="6" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" uniqueName="7" name="Loser2" queryTableFieldId="7" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" uniqueName="8" name="Loser3" queryTableFieldId="8" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" uniqueName="9" name="Loser4" queryTableFieldId="9" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" uniqueName="10" name="Loser5" queryTableFieldId="10" dataDxfId="1"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" uniqueName="11" name="K" queryTableFieldId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1210,35 +1215,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1246,7 +1258,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1254,7 +1266,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1262,7 +1274,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1270,7 +1282,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1278,7 +1290,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1286,7 +1298,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1294,7 +1306,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1302,7 +1314,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1310,7 +1322,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1318,7 +1330,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1326,7 +1338,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1334,7 +1346,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1342,7 +1354,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1490,7 +1502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+    <sheetView topLeftCell="A133" workbookViewId="0">
       <selection activeCell="K165" sqref="K165"/>
     </sheetView>
   </sheetViews>

</xml_diff>